<commit_message>
update EDA file, Create data cleansing file
</commit_message>
<xml_diff>
--- a/data/data_protocol/Employee_Attrition_Max.xlsx
+++ b/data/data_protocol/Employee_Attrition_Max.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,31 +461,11 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Number of Promotions</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
           <t>Distance from Home</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B4" t="n">
         <v>99</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>Number of Dependents</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>